<commit_message>
change on OBQ44 folder name
</commit_message>
<xml_diff>
--- a/scoring/tests/OBQ44/OBQ44_test_2.xlsx
+++ b/scoring/tests/OBQ44/OBQ44_test_2.xlsx
@@ -885,7 +885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,50 +908,60 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>general</t>
+          <t>raw</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>perfectionism/certainty</t>
+          <t>general</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>responsibility_and_threat_estimation</t>
+          <t>perfectionism_certainty</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>importance_and_control_of_thought</t>
+          <t>responsibility_and_threat_estimation</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>importance_and_control_of_thought</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>complete_performance</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>